<commit_message>
Adding view nutrition record feature in user
</commit_message>
<xml_diff>
--- a/Report_Data_Pasien.xlsx
+++ b/Report_Data_Pasien.xlsx
@@ -56,7 +56,7 @@
     <t>Steffan</t>
   </si>
   <si>
-    <t>normal</t>
+    <t>obese</t>
   </si>
   <si>
     <t>Bagus sekali</t>
@@ -514,10 +514,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>12.4</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1">
-        <v>1200</v>
+        <v>150</v>
       </c>
       <c r="F2" s="1">
         <v>12</v>
@@ -555,7 +555,7 @@
         <v>55</v>
       </c>
       <c r="E3" s="1">
-        <v>15000</v>
+        <v>150</v>
       </c>
       <c r="F3" s="1">
         <v>12.3</v>
@@ -593,7 +593,7 @@
         <v>81</v>
       </c>
       <c r="E4" s="1">
-        <v>178</v>
+        <v>1.78</v>
       </c>
       <c r="F4" s="1">
         <v>12</v>
@@ -631,7 +631,7 @@
         <v>60</v>
       </c>
       <c r="E5" s="1">
-        <v>184</v>
+        <v>1.84</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -669,7 +669,7 @@
         <v>78</v>
       </c>
       <c r="E6" s="1">
-        <v>178</v>
+        <v>1.78</v>
       </c>
       <c r="F6" s="1">
         <v>12</v>
@@ -707,7 +707,7 @@
         <v>69</v>
       </c>
       <c r="E7" s="1">
-        <v>169</v>
+        <v>1.69</v>
       </c>
       <c r="F7" s="1">
         <v>23</v>
@@ -745,7 +745,7 @@
         <v>90</v>
       </c>
       <c r="E8" s="1">
-        <v>194</v>
+        <v>1.94</v>
       </c>
       <c r="F8" s="1">
         <v>12</v>
@@ -763,7 +763,7 @@
         <v>100</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>28</v>

</xml_diff>